<commit_message>
receiver ESC control (throttle)
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D31A9514-F02A-4ADC-897E-1137E7777D01}"/>
+  <xr:revisionPtr revIDLastSave="355" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{671D806E-A1AB-42A1-936C-A65E62B0BA7F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Name:</t>
   </si>
@@ -250,6 +250,39 @@
   </si>
   <si>
     <t>I.Bus calibration + Error Handler for Sensor Errors</t>
+  </si>
+  <si>
+    <t>S.Bus decoding</t>
+  </si>
+  <si>
+    <t>Besprechung über Hardwarekonfiguration</t>
+  </si>
+  <si>
+    <t>MPU9250 I2C Kommunikation mit DMA</t>
+  </si>
+  <si>
+    <t>MPU9250 complimentary filter testing</t>
+  </si>
+  <si>
+    <t>MPU9250 complimentary filter better (mit Timer2)</t>
+  </si>
+  <si>
+    <t>Teambesprechung über Jetztstand, Zukunftspläne, Budgetkalkulation und Bestellungen</t>
+  </si>
+  <si>
+    <t>Hardware-Schaltungen-, Printplatten-Design-Besprechung</t>
+  </si>
+  <si>
+    <t>Timer PWM output für ESC, init + duty cycle testing</t>
+  </si>
+  <si>
+    <t>PWM output safemode, throttle control</t>
+  </si>
+  <si>
+    <t>PWM pitch control</t>
+  </si>
+  <si>
+    <t>PWM roll control</t>
   </si>
 </sst>
 </file>
@@ -1337,13 +1370,13 @@
                   <c:v>1.4333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>7.0666666666666673</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>6.1166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2046,19 +2079,20 @@
   </sheetPr>
   <dimension ref="A1:HZ203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="7" style="7" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="83.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
@@ -2087,13 +2121,13 @@
         <f>SUM(E5:E203)</f>
         <v>27.13</v>
       </c>
-      <c r="F2" s="25" t="e">
+      <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G2" s="26" t="e">
+        <v>31.72</v>
+      </c>
+      <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>#NUM!</v>
+        <v>58.84999999999998</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -3155,207 +3189,313 @@
       <c r="C32" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30" t="e">
+      <c r="D32" s="13">
+        <v>0.46597222222222223</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="30">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G32" s="29" t="e">
+        <v>1.1833333333333333</v>
+      </c>
+      <c r="G32" s="29">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H32" s="16"/>
+        <v>1.1833333333333333</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="11" t="e">
+      <c r="A33" s="15">
+        <v>45145</v>
+      </c>
+      <c r="B33" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.84236111111111101</v>
+      </c>
+      <c r="D33" s="13">
+        <v>0.87916666666666676</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
       <c r="F33" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="G33" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="16"/>
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="11" t="e">
+      <c r="A34" s="15">
+        <v>45146</v>
+      </c>
+      <c r="B34" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0.79236111111111107</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
       <c r="F34" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G34" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H34" s="16"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="11" t="e">
+      <c r="A35" s="15">
+        <v>45147</v>
+      </c>
+      <c r="B35" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="D35" s="13">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="E35" s="30">
+        <v>0</v>
+      </c>
       <c r="F35" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1166666666666667</v>
       </c>
       <c r="G35" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="16"/>
+        <v>1.1166666666666667</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="11" t="e">
+      <c r="A36" s="15">
+        <v>45148</v>
+      </c>
+      <c r="B36" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0.66041666666666665</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0.68333333333333324</v>
+      </c>
+      <c r="E36" s="30">
+        <v>0</v>
+      </c>
       <c r="F36" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G36" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="16"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="11" t="e">
+      <c r="A37" s="15">
+        <v>45157</v>
+      </c>
+      <c r="B37" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="C37" s="12">
+        <v>0.875</v>
+      </c>
+      <c r="D37" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E37" s="30">
+        <v>0</v>
+      </c>
       <c r="F37" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G37" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="11" t="e">
+      <c r="A38" s="15">
+        <v>45159</v>
+      </c>
+      <c r="B38" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0.60347222222222219</v>
+      </c>
+      <c r="D38" s="13">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="E38" s="30">
+        <v>0</v>
+      </c>
       <c r="F38" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6166666666666667</v>
       </c>
       <c r="G38" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="16"/>
+        <v>1.6166666666666667</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="11" t="e">
+      <c r="A39" s="15">
+        <v>45162</v>
+      </c>
+      <c r="B39" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C39" s="12">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="D39" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E39" s="30">
+        <v>0</v>
+      </c>
       <c r="F39" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G39" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H39" s="16"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="11" t="e">
+      <c r="A40" s="15">
+        <v>45164</v>
+      </c>
+      <c r="B40" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0.63263888888888886</v>
+      </c>
+      <c r="E40" s="30">
+        <v>0</v>
+      </c>
       <c r="F40" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G40" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="16"/>
+        <v>1.6</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="11" t="e">
+      <c r="A41" s="15">
+        <v>45164</v>
+      </c>
+      <c r="B41" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C41" s="12">
+        <v>0.67499999999999993</v>
+      </c>
+      <c r="D41" s="13">
+        <v>0.73819444444444438</v>
+      </c>
+      <c r="E41" s="30">
+        <v>0</v>
+      </c>
       <c r="F41" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5166666666666666</v>
       </c>
       <c r="G41" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H41" s="16"/>
+        <v>1.5166666666666666</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="11" t="e">
+      <c r="A42" s="15">
+        <v>45164</v>
+      </c>
+      <c r="B42" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C42" s="12">
+        <v>0.83819444444444446</v>
+      </c>
+      <c r="D42" s="13">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E42" s="30">
+        <v>0</v>
+      </c>
       <c r="F42" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21666666666666667</v>
       </c>
       <c r="G42" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H42" s="16"/>
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
@@ -6666,7 +6806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C8:H63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -6680,9 +6820,9 @@
         <v>1</v>
       </c>
       <c r="D8" s="60"/>
-      <c r="E8" s="1" t="e">
+      <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>#NUM!</v>
+        <v>58.85</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -6841,9 +6981,9 @@
       <c r="C27" s="5">
         <v>32</v>
       </c>
-      <c r="D27" s="3" t="e">
+      <c r="D27" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C27,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>#NUM!</v>
+        <v>7.0666666666666673</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
@@ -6852,7 +6992,7 @@
       </c>
       <c r="D28" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C28,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
@@ -6861,7 +7001,7 @@
       </c>
       <c r="D29" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C29,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>6.1166666666666663</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ibus connection test V1 (doesnt work)
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="477" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{251B64FC-4F4A-4F41-8B21-942733C7ECAD}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{746137AC-9903-4CD1-9101-55A45F161479}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>Name:</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>Motor test implementiert</t>
+  </si>
+  <si>
+    <t>IBUS failsafe testen, Platinen bestücken, Programmoptimierungen</t>
+  </si>
+  <si>
+    <t>DS4238 and Receiver Programm Optimisatoinen</t>
+  </si>
+  <si>
+    <t>µC-Platine test, ESC test, test programme entwickelt, IBUS signal lost test</t>
+  </si>
+  <si>
+    <t>DA Besprechung Platinentest</t>
   </si>
 </sst>
 </file>
@@ -1433,10 +1445,10 @@
                   <c:v>10.216666666666667</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.2</c:v>
+                  <c:v>10.533333333333333</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>7.4166666666666661</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -1769,6 +1781,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2125,8 +2141,8 @@
   <dimension ref="A1:HZ203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+      <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,15 +2180,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>33.46</v>
+        <v>42.45</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>59.573333333333338</v>
+        <v>63.333333333333343</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>93.033333333333317</v>
+        <v>105.7833333333333</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -4008,80 +4024,121 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="11" t="e">
+      <c r="A59" s="15">
+        <v>45191</v>
+      </c>
+      <c r="B59" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="30"/>
+        <v>38</v>
+      </c>
+      <c r="C59" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D59" s="13">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E59" s="30">
+        <v>4.49</v>
+      </c>
       <c r="F59" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.84333333333333282</v>
       </c>
       <c r="G59" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H59" s="16"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="11" t="e">
+      <c r="A60" s="15">
+        <v>45196</v>
+      </c>
+      <c r="B60" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C60" s="12">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D60" s="13">
+        <v>0.40625</v>
+      </c>
+      <c r="E60" s="30">
+        <v>0</v>
+      </c>
       <c r="F60" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="G60" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H60" s="16"/>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="H60" s="16" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="B61" s="11" t="e">
+      <c r="A61" s="15">
+        <v>45198</v>
+      </c>
+      <c r="B61" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C61" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E61" s="30">
+        <f>G61-5/6</f>
+        <v>4.5</v>
+      </c>
       <c r="F61" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="G61" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H61" s="16"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="11" t="e">
+      <c r="A62" s="15">
+        <v>45200</v>
+      </c>
+      <c r="B62" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C62" s="12">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D62" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="E62" s="30">
+        <v>0</v>
+      </c>
       <c r="F62" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H62" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
@@ -7028,7 +7085,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>93.033333333333331</v>
+        <v>105.78333333333333</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -7243,7 +7300,7 @@
       </c>
       <c r="D33" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C33,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>5.2</v>
+        <v>10.533333333333333</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
@@ -7252,7 +7309,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C34,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>7.4166666666666661</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
@@ -7528,21 +7585,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -7674,24 +7716,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7707,4 +7747,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new imu breakout added
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="517" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{816BD4D7-83F9-4EE8-9C24-A2FD30471DF6}"/>
+  <xr:revisionPtr revIDLastSave="533" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65451568-0BB6-4996-A096-5E8AA6CD7E9C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
   <si>
     <t>Name:</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Flussdiagramm Erstellung</t>
+  </si>
+  <si>
+    <t>Fehlerbehebung, uC-Platine testen</t>
+  </si>
+  <si>
+    <t>Besprechung Zukunftspläne, Bestellungen, Geld-Management</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1460,7 @@
                   <c:v>7.4166666666666661</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.2833333333333332</c:v>
+                  <c:v>12.116666666666667</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -2145,7 +2151,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,15 +2189,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>42.45</v>
+        <v>46.95</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>68.616666666666674</v>
+        <v>70.95</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>111.06666666666663</v>
+        <v>117.89999999999996</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -4231,42 +4237,62 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="11" t="e">
+      <c r="A66" s="15">
+        <v>45205</v>
+      </c>
+      <c r="B66" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="C66" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D66" s="13">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E66" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F66" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="G66" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H66" s="16"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="H66" s="16" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="11" t="e">
+      <c r="A67" s="15">
+        <v>45205</v>
+      </c>
+      <c r="B67" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="C67" s="12">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D67" s="13">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E67" s="30">
+        <v>0</v>
+      </c>
       <c r="F67" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G67" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H67" s="16"/>
+        <v>1.5</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
@@ -7118,7 +7144,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>111.06666666666666</v>
+        <v>117.9</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -7351,7 +7377,7 @@
       </c>
       <c r="D35" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C35,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>5.2833333333333332</v>
+        <v>12.116666666666667</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
@@ -7618,21 +7644,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -7764,24 +7775,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7797,4 +7806,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sbus and Ibus fix
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="533" documentId="11_244DF2A5C81B934B5237CC8EA0FD7D26E8B2E7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65451568-0BB6-4996-A096-5E8AA6CD7E9C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{656898B4-3387-48F9-A3AA-96D45736039C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="94">
   <si>
     <t>Name:</t>
   </si>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>Besprechung Zukunftspläne, Bestellungen, Geld-Management</t>
+  </si>
+  <si>
+    <t>Lastenheft erstellen</t>
+  </si>
+  <si>
+    <t>IBUS Fehlerkorrektur, M7 Platine testen, Sponsorbesprechung</t>
+  </si>
+  <si>
+    <t>Versuch Fehler zu lösen</t>
+  </si>
+  <si>
+    <t>I.Bus falsche daten fix, S.Bus konfiguration testen</t>
   </si>
 </sst>
 </file>
@@ -1463,10 +1475,10 @@
                   <c:v>12.116666666666667</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>10.883333333333333</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2149,9 +2161,9 @@
   </sheetPr>
   <dimension ref="A1:HZ203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,15 +2201,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>46.95</v>
+        <v>51.45</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>70.95</v>
+        <v>80.833333333333343</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>117.89999999999996</v>
+        <v>132.2833333333333</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -4295,80 +4307,120 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="11" t="e">
+      <c r="A68" s="15">
+        <v>45208</v>
+      </c>
+      <c r="B68" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="30"/>
+        <v>41</v>
+      </c>
+      <c r="C68" s="12">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D68" s="13">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E68" s="30">
+        <v>0</v>
+      </c>
       <c r="F68" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="G68" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H68" s="16"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="11" t="e">
+      <c r="A69" s="15">
+        <v>45212</v>
+      </c>
+      <c r="B69" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C69" s="12"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="30"/>
+        <v>41</v>
+      </c>
+      <c r="C69" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D69" s="13">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E69" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F69" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="G69" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H69" s="16"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="H69" s="16" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="11" t="e">
+      <c r="A70" s="15">
+        <v>45213</v>
+      </c>
+      <c r="B70" s="11">
         <f t="shared" ref="B70:B133" si="3">TRUNC((A70-DATE(YEAR(A70+3-MOD(A70-2,7)),1,MOD(A70-2,7)-9))/7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="30"/>
+        <v>41</v>
+      </c>
+      <c r="C70" s="12">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D70" s="13">
+        <v>0.75208333333333333</v>
+      </c>
+      <c r="E70" s="30">
+        <v>0</v>
+      </c>
       <c r="F70" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.8833333333333333</v>
       </c>
       <c r="G70" s="29">
         <f t="shared" ref="G70:G133" si="4">HOUR($D70-$C70)+MINUTE($D70-$C70)/60</f>
-        <v>0</v>
-      </c>
-      <c r="H70" s="16"/>
+        <v>3.8833333333333333</v>
+      </c>
+      <c r="H70" s="16" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="11" t="e">
+      <c r="A71" s="15">
+        <v>45217</v>
+      </c>
+      <c r="B71" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="30"/>
+        <v>42</v>
+      </c>
+      <c r="C71" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D71" s="13">
+        <v>0.5625</v>
+      </c>
+      <c r="E71" s="30">
+        <v>0</v>
+      </c>
       <c r="F71" s="30">
         <f t="shared" ref="F71:F134" si="5">G71-E71</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="G71" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H71" s="16"/>
+        <v>3.5</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
@@ -7144,7 +7196,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>117.9</v>
+        <v>132.28333333333333</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -7386,7 +7438,7 @@
       </c>
       <c r="D36" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C36,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>10.883333333333333</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
@@ -7395,7 +7447,7 @@
       </c>
       <c r="D37" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C37,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
@@ -7644,6 +7696,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -7775,22 +7842,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7806,21 +7875,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
nach tag der offenen tuer
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D49AAFA6-8A06-4BB1-92D4-20A21BFC9FD6}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0861EDF0-DD9C-47A0-8B20-328079792DAE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Begleitprotokoll" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
   <si>
     <t>Name:</t>
   </si>
@@ -391,6 +391,21 @@
   </si>
   <si>
     <t>DS2438 Fehlerbehebung</t>
+  </si>
+  <si>
+    <t>Einlesen in X-Cube MEMS1</t>
+  </si>
+  <si>
+    <t>Testen</t>
+  </si>
+  <si>
+    <t>MPU9250 Daten Visualierung</t>
+  </si>
+  <si>
+    <t>MPU9250 Magnetometer Kommunikation Test + Tag der offenen Tür Programm fertig gestellt</t>
+  </si>
+  <si>
+    <t>Motorentest, Vorbereitungen Tag der offenen Tür</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1535,10 @@
                   <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>20.283333333333331</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -1832,6 +1847,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2188,23 +2207,23 @@
   <dimension ref="A1:HZ203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
+      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:234" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -2218,7 +2237,7 @@
       <c r="G1" s="41"/>
       <c r="H1" s="42"/>
     </row>
-    <row r="2" spans="1:234" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
@@ -2227,19 +2246,19 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>60.45</v>
-      </c>
-      <c r="F2" s="25" t="e">
+        <v>64.95</v>
+      </c>
+      <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G2" s="26" t="e">
+        <v>108.4</v>
+      </c>
+      <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>#NUM!</v>
+        <v>173.35</v>
       </c>
       <c r="H2" s="27"/>
     </row>
-    <row r="3" spans="1:234" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:234" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
@@ -2489,7 +2508,7 @@
       <c r="HY3" s="7"/>
       <c r="HZ3" s="7"/>
     </row>
-    <row r="4" spans="1:234" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="42"/>
       <c r="B4" s="44"/>
       <c r="C4" s="28" t="s">
@@ -2503,7 +2522,7 @@
       <c r="G4" s="47"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>45056</v>
       </c>
@@ -2532,7 +2551,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>45063</v>
       </c>
@@ -2561,7 +2580,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>45069</v>
       </c>
@@ -2591,7 +2610,7 @@
       </c>
       <c r="J7" s="23"/>
     </row>
-    <row r="8" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>45070</v>
       </c>
@@ -2620,7 +2639,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:234" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:234" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>45077</v>
       </c>
@@ -2649,7 +2668,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>45091</v>
       </c>
@@ -2678,7 +2697,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>45091</v>
       </c>
@@ -2707,7 +2726,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>45093</v>
       </c>
@@ -2736,7 +2755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>45094</v>
       </c>
@@ -2765,7 +2784,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>45098</v>
       </c>
@@ -2794,7 +2813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>45103</v>
       </c>
@@ -2823,7 +2842,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:234" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>45103</v>
       </c>
@@ -2852,7 +2871,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>45104</v>
       </c>
@@ -2881,7 +2900,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>45111</v>
       </c>
@@ -2910,7 +2929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>45112</v>
       </c>
@@ -2939,7 +2958,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>45118</v>
       </c>
@@ -2968,7 +2987,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>45118</v>
       </c>
@@ -2997,7 +3016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>45125</v>
       </c>
@@ -3026,7 +3045,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>45126</v>
       </c>
@@ -3055,7 +3074,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>45131</v>
       </c>
@@ -3084,7 +3103,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>45132</v>
       </c>
@@ -3113,7 +3132,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>45132</v>
       </c>
@@ -3142,7 +3161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>45133</v>
       </c>
@@ -3171,7 +3190,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>45136</v>
       </c>
@@ -3200,7 +3219,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>45137</v>
       </c>
@@ -3229,7 +3248,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <v>45137</v>
       </c>
@@ -3258,7 +3277,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>45141</v>
       </c>
@@ -3287,7 +3306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>45145</v>
       </c>
@@ -3316,7 +3335,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>45145</v>
       </c>
@@ -3345,7 +3364,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>45146</v>
       </c>
@@ -3374,7 +3393,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <v>45147</v>
       </c>
@@ -3403,7 +3422,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>45148</v>
       </c>
@@ -3432,7 +3451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>45157</v>
       </c>
@@ -3461,7 +3480,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>45159</v>
       </c>
@@ -3490,7 +3509,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>45162</v>
       </c>
@@ -3519,7 +3538,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <v>45164</v>
       </c>
@@ -3548,7 +3567,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <v>45164</v>
       </c>
@@ -3577,7 +3596,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <v>45164</v>
       </c>
@@ -3606,7 +3625,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>45165</v>
       </c>
@@ -3635,7 +3654,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>45168</v>
       </c>
@@ -3664,7 +3683,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>45171</v>
       </c>
@@ -3693,7 +3712,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <v>45176</v>
       </c>
@@ -3722,7 +3741,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
         <v>45177</v>
       </c>
@@ -3751,7 +3770,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <v>45179</v>
       </c>
@@ -3780,7 +3799,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="15">
         <v>45180</v>
       </c>
@@ -3809,7 +3828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="15">
         <v>45181</v>
       </c>
@@ -3838,7 +3857,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="15">
         <v>45182</v>
       </c>
@@ -3867,7 +3886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <v>45182</v>
       </c>
@@ -3896,7 +3915,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15">
         <v>45184</v>
       </c>
@@ -3925,7 +3944,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <v>45185</v>
       </c>
@@ -3954,7 +3973,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>45187</v>
       </c>
@@ -3983,7 +4002,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>45187</v>
       </c>
@@ -4012,7 +4031,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>45189</v>
       </c>
@@ -4041,7 +4060,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="15">
         <v>45190</v>
       </c>
@@ -4070,7 +4089,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="15">
         <v>45191</v>
       </c>
@@ -4099,7 +4118,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>45196</v>
       </c>
@@ -4128,7 +4147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="15">
         <v>45198</v>
       </c>
@@ -4158,7 +4177,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>45200</v>
       </c>
@@ -4187,7 +4206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>45201</v>
       </c>
@@ -4216,7 +4235,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>45201</v>
       </c>
@@ -4245,7 +4264,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>45202</v>
       </c>
@@ -4274,7 +4293,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>45205</v>
       </c>
@@ -4303,7 +4322,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <v>45205</v>
       </c>
@@ -4332,7 +4351,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>45208</v>
       </c>
@@ -4361,7 +4380,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <v>45212</v>
       </c>
@@ -4390,7 +4409,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <v>45213</v>
       </c>
@@ -4419,7 +4438,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <v>45217</v>
       </c>
@@ -4448,7 +4467,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="15">
         <v>45219</v>
       </c>
@@ -4477,7 +4496,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="15">
         <v>45236</v>
       </c>
@@ -4506,7 +4525,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>45240</v>
       </c>
@@ -4535,7 +4554,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="15">
         <v>45243</v>
       </c>
@@ -4564,7 +4583,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="15">
         <v>45245</v>
       </c>
@@ -4593,7 +4612,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="15">
         <v>45245</v>
       </c>
@@ -4622,7 +4641,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="15">
         <v>45246</v>
       </c>
@@ -4651,7 +4670,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>45246</v>
       </c>
@@ -4680,7 +4699,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="15">
         <v>45247</v>
       </c>
@@ -4709,7 +4728,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="15">
         <v>45247</v>
       </c>
@@ -4738,7 +4757,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="15">
         <v>45248</v>
       </c>
@@ -4749,95 +4768,141 @@
       <c r="C82" s="12">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30" t="e">
+      <c r="D82" s="13">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="E82" s="30">
+        <v>0</v>
+      </c>
+      <c r="F82" s="30">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G82" s="29" t="e">
+        <v>1.8833333333333333</v>
+      </c>
+      <c r="G82" s="29">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H82" s="16"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
-      <c r="B83" s="11" t="e">
+        <v>1.8833333333333333</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="15">
+        <v>45249</v>
+      </c>
+      <c r="B83" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="C83" s="12">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D83" s="13">
+        <v>0.45416666666666666</v>
+      </c>
+      <c r="E83" s="30">
+        <v>0</v>
+      </c>
       <c r="F83" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="G83" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H83" s="16"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-      <c r="B84" s="11" t="e">
+        <v>0.65</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="15">
+        <v>45250</v>
+      </c>
+      <c r="B84" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="C84" s="12">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D84" s="13">
+        <v>0.90625</v>
+      </c>
+      <c r="E84" s="30">
+        <v>0</v>
+      </c>
       <c r="F84" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4166666666666665</v>
       </c>
       <c r="G84" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H84" s="16"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="11" t="e">
+        <v>3.4166666666666665</v>
+      </c>
+      <c r="H84" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="15">
+        <v>45251</v>
+      </c>
+      <c r="B85" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="C85" s="12">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D85" s="13">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E85" s="30">
+        <v>0</v>
+      </c>
       <c r="F85" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G85" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H85" s="16"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="11" t="e">
+        <v>3</v>
+      </c>
+      <c r="H85" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="15">
+        <v>45254</v>
+      </c>
+      <c r="B86" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="C86" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D86" s="13">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E86" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F86" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="G86" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H86" s="16"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="H86" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="15"/>
       <c r="B87" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4856,7 +4921,7 @@
       </c>
       <c r="H87" s="16"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="15"/>
       <c r="B88" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4875,7 +4940,7 @@
       </c>
       <c r="H88" s="16"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="15"/>
       <c r="B89" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4894,7 +4959,7 @@
       </c>
       <c r="H89" s="16"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="15"/>
       <c r="B90" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4913,7 +4978,7 @@
       </c>
       <c r="H90" s="16"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="15"/>
       <c r="B91" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4932,7 +4997,7 @@
       </c>
       <c r="H91" s="16"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="15"/>
       <c r="B92" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4951,7 +5016,7 @@
       </c>
       <c r="H92" s="16"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="15"/>
       <c r="B93" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4970,7 +5035,7 @@
       </c>
       <c r="H93" s="16"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="15"/>
       <c r="B94" s="11" t="e">
         <f t="shared" si="3"/>
@@ -4989,7 +5054,7 @@
       </c>
       <c r="H94" s="16"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="15"/>
       <c r="B95" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5008,7 +5073,7 @@
       </c>
       <c r="H95" s="16"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="15"/>
       <c r="B96" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5027,7 +5092,7 @@
       </c>
       <c r="H96" s="16"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="15"/>
       <c r="B97" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5046,7 +5111,7 @@
       </c>
       <c r="H97" s="16"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="15"/>
       <c r="B98" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5065,7 +5130,7 @@
       </c>
       <c r="H98" s="16"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="15"/>
       <c r="B99" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5084,7 +5149,7 @@
       </c>
       <c r="H99" s="16"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="15"/>
       <c r="B100" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5103,7 +5168,7 @@
       </c>
       <c r="H100" s="16"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="15"/>
       <c r="B101" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5122,7 +5187,7 @@
       </c>
       <c r="H101" s="17"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="15"/>
       <c r="B102" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5141,7 +5206,7 @@
       </c>
       <c r="H102" s="16"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="15"/>
       <c r="B103" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5160,7 +5225,7 @@
       </c>
       <c r="H103" s="16"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="15"/>
       <c r="B104" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5179,7 +5244,7 @@
       </c>
       <c r="H104" s="16"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="15"/>
       <c r="B105" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5198,7 +5263,7 @@
       </c>
       <c r="H105" s="16"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="15"/>
       <c r="B106" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5217,7 +5282,7 @@
       </c>
       <c r="H106" s="16"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="15"/>
       <c r="B107" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5236,7 +5301,7 @@
       </c>
       <c r="H107" s="16"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="15"/>
       <c r="B108" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5255,7 +5320,7 @@
       </c>
       <c r="H108" s="16"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="15"/>
       <c r="B109" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5274,7 +5339,7 @@
       </c>
       <c r="H109" s="16"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="15"/>
       <c r="B110" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5293,7 +5358,7 @@
       </c>
       <c r="H110" s="16"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="15"/>
       <c r="B111" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5312,7 +5377,7 @@
       </c>
       <c r="H111" s="16"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="15"/>
       <c r="B112" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5331,7 +5396,7 @@
       </c>
       <c r="H112" s="16"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="15"/>
       <c r="B113" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5350,7 +5415,7 @@
       </c>
       <c r="H113" s="16"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="15"/>
       <c r="B114" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5369,7 +5434,7 @@
       </c>
       <c r="H114" s="16"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="15"/>
       <c r="B115" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5388,7 +5453,7 @@
       </c>
       <c r="H115" s="16"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="15"/>
       <c r="B116" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5407,7 +5472,7 @@
       </c>
       <c r="H116" s="16"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="15"/>
       <c r="B117" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5426,7 +5491,7 @@
       </c>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="15"/>
       <c r="B118" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5445,7 +5510,7 @@
       </c>
       <c r="H118" s="16"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="15"/>
       <c r="B119" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5464,7 +5529,7 @@
       </c>
       <c r="H119" s="16"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="15"/>
       <c r="B120" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5483,7 +5548,7 @@
       </c>
       <c r="H120" s="16"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="15"/>
       <c r="B121" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5502,7 +5567,7 @@
       </c>
       <c r="H121" s="16"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="15"/>
       <c r="B122" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5521,7 +5586,7 @@
       </c>
       <c r="H122" s="16"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="15"/>
       <c r="B123" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5540,7 +5605,7 @@
       </c>
       <c r="H123" s="16"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="15"/>
       <c r="B124" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5559,7 +5624,7 @@
       </c>
       <c r="H124" s="16"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="15"/>
       <c r="B125" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5578,7 +5643,7 @@
       </c>
       <c r="H125" s="16"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="15"/>
       <c r="B126" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5597,7 +5662,7 @@
       </c>
       <c r="H126" s="16"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="15"/>
       <c r="B127" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5616,7 +5681,7 @@
       </c>
       <c r="H127" s="16"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="15"/>
       <c r="B128" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5635,7 +5700,7 @@
       </c>
       <c r="H128" s="16"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="15"/>
       <c r="B129" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5654,7 +5719,7 @@
       </c>
       <c r="H129" s="16"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="15"/>
       <c r="B130" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5673,7 +5738,7 @@
       </c>
       <c r="H130" s="16"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="15"/>
       <c r="B131" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5692,7 +5757,7 @@
       </c>
       <c r="H131" s="16"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="15"/>
       <c r="B132" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5711,7 +5776,7 @@
       </c>
       <c r="H132" s="16"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="15"/>
       <c r="B133" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5730,7 +5795,7 @@
       </c>
       <c r="H133" s="16"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="15"/>
       <c r="B134" s="11" t="e">
         <f t="shared" ref="B134:B197" si="6">TRUNC((A134-DATE(YEAR(A134+3-MOD(A134-2,7)),1,MOD(A134-2,7)-9))/7)</f>
@@ -5749,7 +5814,7 @@
       </c>
       <c r="H134" s="16"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="15"/>
       <c r="B135" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5768,7 +5833,7 @@
       </c>
       <c r="H135" s="16"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="15"/>
       <c r="B136" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5787,7 +5852,7 @@
       </c>
       <c r="H136" s="16"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="15"/>
       <c r="B137" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5806,7 +5871,7 @@
       </c>
       <c r="H137" s="16"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="15"/>
       <c r="B138" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5825,7 +5890,7 @@
       </c>
       <c r="H138" s="16"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="15"/>
       <c r="B139" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5844,7 +5909,7 @@
       </c>
       <c r="H139" s="16"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="15"/>
       <c r="B140" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5863,7 +5928,7 @@
       </c>
       <c r="H140" s="16"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="15"/>
       <c r="B141" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5882,7 +5947,7 @@
       </c>
       <c r="H141" s="16"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="15"/>
       <c r="B142" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5901,7 +5966,7 @@
       </c>
       <c r="H142" s="16"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="15"/>
       <c r="B143" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5920,7 +5985,7 @@
       </c>
       <c r="H143" s="16"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="15"/>
       <c r="B144" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5939,7 +6004,7 @@
       </c>
       <c r="H144" s="16"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="15"/>
       <c r="B145" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5958,7 +6023,7 @@
       </c>
       <c r="H145" s="16"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="15"/>
       <c r="B146" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5977,7 +6042,7 @@
       </c>
       <c r="H146" s="16"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="15"/>
       <c r="B147" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5996,7 +6061,7 @@
       </c>
       <c r="H147" s="16"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="15"/>
       <c r="B148" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6015,7 +6080,7 @@
       </c>
       <c r="H148" s="16"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="15"/>
       <c r="B149" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6034,7 +6099,7 @@
       </c>
       <c r="H149" s="16"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="15"/>
       <c r="B150" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6053,7 +6118,7 @@
       </c>
       <c r="H150" s="16"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="15"/>
       <c r="B151" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6072,7 +6137,7 @@
       </c>
       <c r="H151" s="16"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="15"/>
       <c r="B152" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6091,7 +6156,7 @@
       </c>
       <c r="H152" s="16"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="15"/>
       <c r="B153" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6110,7 +6175,7 @@
       </c>
       <c r="H153" s="16"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="15"/>
       <c r="B154" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6129,7 +6194,7 @@
       </c>
       <c r="H154" s="16"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="15"/>
       <c r="B155" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6148,7 +6213,7 @@
       </c>
       <c r="H155" s="16"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="15"/>
       <c r="B156" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6167,7 +6232,7 @@
       </c>
       <c r="H156" s="16"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="15"/>
       <c r="B157" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6186,7 +6251,7 @@
       </c>
       <c r="H157" s="16"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="15"/>
       <c r="B158" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6205,7 +6270,7 @@
       </c>
       <c r="H158" s="16"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="15"/>
       <c r="B159" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6224,7 +6289,7 @@
       </c>
       <c r="H159" s="16"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="15"/>
       <c r="B160" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6243,7 +6308,7 @@
       </c>
       <c r="H160" s="16"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="15"/>
       <c r="B161" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6262,7 +6327,7 @@
       </c>
       <c r="H161" s="16"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="15"/>
       <c r="B162" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6281,7 +6346,7 @@
       </c>
       <c r="H162" s="16"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="15"/>
       <c r="B163" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6300,7 +6365,7 @@
       </c>
       <c r="H163" s="16"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="15"/>
       <c r="B164" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6319,7 +6384,7 @@
       </c>
       <c r="H164" s="16"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="15"/>
       <c r="B165" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6338,7 +6403,7 @@
       </c>
       <c r="H165" s="16"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="15"/>
       <c r="B166" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6357,7 +6422,7 @@
       </c>
       <c r="H166" s="16"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="15"/>
       <c r="B167" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6376,7 +6441,7 @@
       </c>
       <c r="H167" s="16"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="15"/>
       <c r="B168" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6395,7 +6460,7 @@
       </c>
       <c r="H168" s="16"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="15"/>
       <c r="B169" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6414,7 +6479,7 @@
       </c>
       <c r="H169" s="16"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="15"/>
       <c r="B170" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6433,7 +6498,7 @@
       </c>
       <c r="H170" s="16"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="15"/>
       <c r="B171" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6452,7 +6517,7 @@
       </c>
       <c r="H171" s="16"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="15"/>
       <c r="B172" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6471,7 +6536,7 @@
       </c>
       <c r="H172" s="16"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="15"/>
       <c r="B173" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6490,7 +6555,7 @@
       </c>
       <c r="H173" s="16"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="15"/>
       <c r="B174" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6509,7 +6574,7 @@
       </c>
       <c r="H174" s="16"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="15"/>
       <c r="B175" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6528,7 +6593,7 @@
       </c>
       <c r="H175" s="16"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="15"/>
       <c r="B176" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6547,7 +6612,7 @@
       </c>
       <c r="H176" s="16"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="15"/>
       <c r="B177" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6566,7 +6631,7 @@
       </c>
       <c r="H177" s="16"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="15"/>
       <c r="B178" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6585,7 +6650,7 @@
       </c>
       <c r="H178" s="16"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="15"/>
       <c r="B179" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6604,7 +6669,7 @@
       </c>
       <c r="H179" s="16"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="15"/>
       <c r="B180" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6623,7 +6688,7 @@
       </c>
       <c r="H180" s="16"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="15"/>
       <c r="B181" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6642,7 +6707,7 @@
       </c>
       <c r="H181" s="16"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="15"/>
       <c r="B182" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6661,7 +6726,7 @@
       </c>
       <c r="H182" s="16"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="15"/>
       <c r="B183" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6680,7 +6745,7 @@
       </c>
       <c r="H183" s="16"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="15"/>
       <c r="B184" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6699,7 +6764,7 @@
       </c>
       <c r="H184" s="16"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="15"/>
       <c r="B185" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6718,7 +6783,7 @@
       </c>
       <c r="H185" s="16"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="15"/>
       <c r="B186" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6737,7 +6802,7 @@
       </c>
       <c r="H186" s="16"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="15"/>
       <c r="B187" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6756,7 +6821,7 @@
       </c>
       <c r="H187" s="16"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="15"/>
       <c r="B188" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6775,7 +6840,7 @@
       </c>
       <c r="H188" s="16"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="15"/>
       <c r="B189" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6794,7 +6859,7 @@
       </c>
       <c r="H189" s="16"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="15"/>
       <c r="B190" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6813,7 +6878,7 @@
       </c>
       <c r="H190" s="16"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="15"/>
       <c r="B191" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6832,7 +6897,7 @@
       </c>
       <c r="H191" s="16"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="15"/>
       <c r="B192" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6851,7 +6916,7 @@
       </c>
       <c r="H192" s="16"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="15"/>
       <c r="B193" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6870,7 +6935,7 @@
       </c>
       <c r="H193" s="16"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="15"/>
       <c r="B194" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6889,7 +6954,7 @@
       </c>
       <c r="H194" s="16"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="15"/>
       <c r="B195" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6908,7 +6973,7 @@
       </c>
       <c r="H195" s="16"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="15"/>
       <c r="B196" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6927,7 +6992,7 @@
       </c>
       <c r="H196" s="16"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="15"/>
       <c r="B197" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6946,7 +7011,7 @@
       </c>
       <c r="H197" s="16"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="15"/>
       <c r="B198" s="11" t="e">
         <f t="shared" ref="B198:B203" si="9">TRUNC((A198-DATE(YEAR(A198+3-MOD(A198-2,7)),1,MOD(A198-2,7)-9))/7)</f>
@@ -6965,7 +7030,7 @@
       </c>
       <c r="H198" s="16"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="15"/>
       <c r="B199" s="11" t="e">
         <f t="shared" si="9"/>
@@ -6984,7 +7049,7 @@
       </c>
       <c r="H199" s="16"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="15"/>
       <c r="B200" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7003,7 +7068,7 @@
       </c>
       <c r="H200" s="16"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="15"/>
       <c r="B201" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7022,7 +7087,7 @@
       </c>
       <c r="H201" s="16"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="15"/>
       <c r="B202" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7041,7 +7106,7 @@
       </c>
       <c r="H202" s="16"/>
     </row>
-    <row r="203" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="18"/>
       <c r="B203" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7093,15 +7158,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" customWidth="1"/>
-    <col min="3" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" customWidth="1"/>
+    <col min="3" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="57" t="s">
         <v>11</v>
       </c>
@@ -7113,7 +7178,7 @@
       <c r="G1" s="57"/>
       <c r="H1" s="57"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7131,7 +7196,7 @@
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
     </row>
-    <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
@@ -7147,7 +7212,7 @@
       <c r="G3" s="59"/>
       <c r="H3" s="59"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -7155,8 +7220,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>17</v>
       </c>
@@ -7182,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="34">
         <v>42900</v>
       </c>
@@ -7204,7 +7269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -7214,7 +7279,7 @@
       <c r="G8" s="36"/>
       <c r="H8" s="38"/>
     </row>
-    <row r="9" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="39"/>
       <c r="C9" s="36"/>
@@ -7224,7 +7289,7 @@
       <c r="G9" s="36"/>
       <c r="H9" s="38"/>
     </row>
-    <row r="10" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" s="35"/>
       <c r="C10" s="36"/>
@@ -7234,7 +7299,7 @@
       <c r="G10" s="36"/>
       <c r="H10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" s="35"/>
       <c r="C11" s="36"/>
@@ -7244,7 +7309,7 @@
       <c r="G11" s="36"/>
       <c r="H11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="36"/>
@@ -7254,8 +7319,8 @@
       <c r="G12" s="36"/>
       <c r="H12" s="38"/>
     </row>
-    <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="50" t="s">
         <v>27</v>
       </c>
@@ -7267,7 +7332,7 @@
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
@@ -7277,7 +7342,7 @@
       <c r="G15" s="52"/>
       <c r="H15" s="53"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="54"/>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -7310,26 +7375,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C8:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="60" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="60"/>
-      <c r="E8" s="1" t="e">
+      <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+        <v>173.35</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
@@ -7337,7 +7402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>16</v>
       </c>
@@ -7346,7 +7411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>17</v>
       </c>
@@ -7355,7 +7420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>18</v>
       </c>
@@ -7364,7 +7429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>19</v>
       </c>
@@ -7373,7 +7438,7 @@
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="5">
         <v>20</v>
       </c>
@@ -7382,7 +7447,7 @@
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>21</v>
       </c>
@@ -7391,7 +7456,7 @@
         <v>4.583333333333333</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>22</v>
       </c>
@@ -7400,7 +7465,7 @@
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>23</v>
       </c>
@@ -7409,7 +7474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>24</v>
       </c>
@@ -7418,7 +7483,7 @@
         <v>5.6833333333333336</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>25</v>
       </c>
@@ -7427,7 +7492,7 @@
         <v>1.4833333333333334</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>26</v>
       </c>
@@ -7436,7 +7501,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>27</v>
       </c>
@@ -7445,7 +7510,7 @@
         <v>1.9333333333333331</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>28</v>
       </c>
@@ -7454,7 +7519,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>29</v>
       </c>
@@ -7463,7 +7528,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>30</v>
       </c>
@@ -7472,7 +7537,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="5">
         <v>31</v>
       </c>
@@ -7481,7 +7546,7 @@
         <v>1.4333333333333333</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" s="5">
         <v>32</v>
       </c>
@@ -7490,7 +7555,7 @@
         <v>7.0666666666666673</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="5">
         <v>33</v>
       </c>
@@ -7499,7 +7564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="5">
         <v>34</v>
       </c>
@@ -7508,7 +7573,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="5">
         <v>35</v>
       </c>
@@ -7517,7 +7582,7 @@
         <v>4.2166666666666668</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="5">
         <v>36</v>
       </c>
@@ -7526,7 +7591,7 @@
         <v>11.566666666666666</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" s="5">
         <v>37</v>
       </c>
@@ -7535,7 +7600,7 @@
         <v>10.216666666666667</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="5">
         <v>38</v>
       </c>
@@ -7544,7 +7609,7 @@
         <v>10.533333333333333</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="5">
         <v>39</v>
       </c>
@@ -7553,7 +7618,7 @@
         <v>7.4166666666666661</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="5">
         <v>40</v>
       </c>
@@ -7562,7 +7627,7 @@
         <v>12.116666666666667</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="5">
         <v>41</v>
       </c>
@@ -7571,7 +7636,7 @@
         <v>10.883333333333333</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
         <v>42</v>
       </c>
@@ -7580,7 +7645,7 @@
         <v>8.8333333333333321</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" s="5">
         <v>43</v>
       </c>
@@ -7589,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" s="5">
         <v>44</v>
       </c>
@@ -7598,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="5">
         <v>45</v>
       </c>
@@ -7607,25 +7672,25 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="5">
         <v>46</v>
       </c>
-      <c r="D41" s="3" t="e">
+      <c r="D41" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C41,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+        <v>20.283333333333331</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" s="5">
         <v>47</v>
       </c>
       <c r="D42" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C42,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" s="5">
         <v>48</v>
       </c>
@@ -7634,7 +7699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" s="5">
         <v>49</v>
       </c>
@@ -7643,7 +7708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" s="5">
         <v>50</v>
       </c>
@@ -7652,7 +7717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" s="5">
         <v>51</v>
       </c>
@@ -7661,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" s="5">
         <v>52</v>
       </c>
@@ -7670,7 +7735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" s="5">
         <v>1</v>
       </c>
@@ -7679,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C49" s="5">
         <v>2</v>
       </c>
@@ -7689,7 +7754,7 @@
       </c>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C50" s="5">
         <v>3</v>
       </c>
@@ -7698,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C51" s="5">
         <v>4</v>
       </c>
@@ -7707,7 +7772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C52" s="5">
         <v>5</v>
       </c>
@@ -7716,7 +7781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C53" s="5">
         <v>6</v>
       </c>
@@ -7725,7 +7790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C54" s="5">
         <v>7</v>
       </c>
@@ -7735,7 +7800,7 @@
       </c>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C55" s="5">
         <v>8</v>
       </c>
@@ -7745,7 +7810,7 @@
       </c>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C56" s="5">
         <v>9</v>
       </c>
@@ -7754,7 +7819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C57" s="5">
         <v>10</v>
       </c>
@@ -7763,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C58" s="5">
         <v>11</v>
       </c>
@@ -7773,7 +7838,7 @@
       </c>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C59" s="5">
         <v>12</v>
       </c>
@@ -7783,7 +7848,7 @@
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C60" s="5">
         <v>13</v>
       </c>
@@ -7792,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C61" s="5">
         <v>14</v>
       </c>
@@ -7801,7 +7866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C62" s="5">
         <v>15</v>
       </c>
@@ -7810,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D63" s="3"/>
     </row>
   </sheetData>
@@ -7826,12 +7891,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7967,15 +8029,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7999,10 +8065,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
dshot nacheinander + imu10dof connection test
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0861EDF0-DD9C-47A0-8B20-328079792DAE}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DA02A0C-33A3-424D-96A4-E91C03C75E89}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Begleitprotokoll" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="114">
   <si>
     <t>Name:</t>
   </si>
@@ -406,6 +406,21 @@
   </si>
   <si>
     <t>Motorentest, Vorbereitungen Tag der offenen Tür</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einlesen in Motorenansteuerung </t>
+  </si>
+  <si>
+    <t>Dshot Protokoll ausprogrammiert</t>
+  </si>
+  <si>
+    <t>Dshot auf 4 Kanäle debuggen</t>
+  </si>
+  <si>
+    <t>Dshot auf alle 4 Kanäle</t>
+  </si>
+  <si>
+    <t>IMU 10DOF connection test</t>
   </si>
 </sst>
 </file>
@@ -1541,10 +1556,10 @@
                   <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -1847,10 +1862,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2208,22 +2219,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H87" sqref="H87"/>
+      <selection pane="bottomLeft" activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:234" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2248,7 @@
       <c r="G1" s="41"/>
       <c r="H1" s="42"/>
     </row>
-    <row r="2" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:234" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
@@ -2246,19 +2257,19 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>64.95</v>
+        <v>69.45</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>108.4</v>
+        <v>119.9</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>173.35</v>
+        <v>189.35</v>
       </c>
       <c r="H2" s="27"/>
     </row>
-    <row r="3" spans="1:234" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:234" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
@@ -2508,7 +2519,7 @@
       <c r="HY3" s="7"/>
       <c r="HZ3" s="7"/>
     </row>
-    <row r="4" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:234" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42"/>
       <c r="B4" s="44"/>
       <c r="C4" s="28" t="s">
@@ -2522,7 +2533,7 @@
       <c r="G4" s="47"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>45056</v>
       </c>
@@ -2551,7 +2562,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>45063</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>45069</v>
       </c>
@@ -2610,7 +2621,7 @@
       </c>
       <c r="J7" s="23"/>
     </row>
-    <row r="8" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>45070</v>
       </c>
@@ -2639,7 +2650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:234" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:234" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>45077</v>
       </c>
@@ -2668,7 +2679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>45091</v>
       </c>
@@ -2697,7 +2708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>45091</v>
       </c>
@@ -2726,7 +2737,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>45093</v>
       </c>
@@ -2755,7 +2766,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>45094</v>
       </c>
@@ -2784,7 +2795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>45098</v>
       </c>
@@ -2813,7 +2824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>45103</v>
       </c>
@@ -2842,7 +2853,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:234" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>45103</v>
       </c>
@@ -2871,7 +2882,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>45104</v>
       </c>
@@ -2900,7 +2911,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>45111</v>
       </c>
@@ -2929,7 +2940,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>45112</v>
       </c>
@@ -2958,7 +2969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>45118</v>
       </c>
@@ -2987,7 +2998,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>45118</v>
       </c>
@@ -3016,7 +3027,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>45125</v>
       </c>
@@ -3045,7 +3056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>45126</v>
       </c>
@@ -3074,7 +3085,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>45131</v>
       </c>
@@ -3103,7 +3114,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>45132</v>
       </c>
@@ -3132,7 +3143,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>45132</v>
       </c>
@@ -3161,7 +3172,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>45133</v>
       </c>
@@ -3190,7 +3201,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>45136</v>
       </c>
@@ -3219,7 +3230,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>45137</v>
       </c>
@@ -3248,7 +3259,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>45137</v>
       </c>
@@ -3277,7 +3288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>45141</v>
       </c>
@@ -3306,7 +3317,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>45145</v>
       </c>
@@ -3335,7 +3346,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>45145</v>
       </c>
@@ -3364,7 +3375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>45146</v>
       </c>
@@ -3393,7 +3404,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>45147</v>
       </c>
@@ -3422,7 +3433,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>45148</v>
       </c>
@@ -3451,7 +3462,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>45157</v>
       </c>
@@ -3480,7 +3491,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>45159</v>
       </c>
@@ -3509,7 +3520,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>45162</v>
       </c>
@@ -3538,7 +3549,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>45164</v>
       </c>
@@ -3567,7 +3578,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>45164</v>
       </c>
@@ -3596,7 +3607,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>45164</v>
       </c>
@@ -3625,7 +3636,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>45165</v>
       </c>
@@ -3654,7 +3665,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>45168</v>
       </c>
@@ -3683,7 +3694,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>45171</v>
       </c>
@@ -3712,7 +3723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45176</v>
       </c>
@@ -3741,7 +3752,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>45177</v>
       </c>
@@ -3770,7 +3781,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>45179</v>
       </c>
@@ -3799,7 +3810,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>45180</v>
       </c>
@@ -3828,7 +3839,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>45181</v>
       </c>
@@ -3857,7 +3868,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>45182</v>
       </c>
@@ -3886,7 +3897,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>45182</v>
       </c>
@@ -3915,7 +3926,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>45184</v>
       </c>
@@ -3944,7 +3955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>45185</v>
       </c>
@@ -3973,7 +3984,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>45187</v>
       </c>
@@ -4002,7 +4013,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>45187</v>
       </c>
@@ -4031,7 +4042,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>45189</v>
       </c>
@@ -4060,7 +4071,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>45190</v>
       </c>
@@ -4089,7 +4100,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>45191</v>
       </c>
@@ -4118,7 +4129,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>45196</v>
       </c>
@@ -4147,7 +4158,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>45198</v>
       </c>
@@ -4177,7 +4188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>45200</v>
       </c>
@@ -4206,7 +4217,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>45201</v>
       </c>
@@ -4235,7 +4246,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>45201</v>
       </c>
@@ -4264,7 +4275,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>45202</v>
       </c>
@@ -4293,7 +4304,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <v>45205</v>
       </c>
@@ -4322,7 +4333,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>45205</v>
       </c>
@@ -4351,7 +4362,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>45208</v>
       </c>
@@ -4380,7 +4391,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>45212</v>
       </c>
@@ -4409,7 +4420,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <v>45213</v>
       </c>
@@ -4438,7 +4449,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>45217</v>
       </c>
@@ -4467,7 +4478,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>45219</v>
       </c>
@@ -4496,7 +4507,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>45236</v>
       </c>
@@ -4525,7 +4536,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <v>45240</v>
       </c>
@@ -4554,7 +4565,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>45243</v>
       </c>
@@ -4583,7 +4594,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>45245</v>
       </c>
@@ -4612,7 +4623,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>45245</v>
       </c>
@@ -4641,7 +4652,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <v>45246</v>
       </c>
@@ -4670,7 +4681,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>45246</v>
       </c>
@@ -4699,7 +4710,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>45247</v>
       </c>
@@ -4728,7 +4739,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>45247</v>
       </c>
@@ -4757,7 +4768,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>45248</v>
       </c>
@@ -4786,7 +4797,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>45249</v>
       </c>
@@ -4815,7 +4826,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <v>45250</v>
       </c>
@@ -4844,7 +4855,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <v>45251</v>
       </c>
@@ -4873,7 +4884,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <v>45254</v>
       </c>
@@ -4902,102 +4913,152 @@
         <v>108</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="15"/>
-      <c r="B87" s="11" t="e">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="15">
+        <v>45260</v>
+      </c>
+      <c r="B87" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C87" s="12"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="C87" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="D87" s="13">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E87" s="30">
+        <v>0</v>
+      </c>
       <c r="F87" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G87" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H87" s="16"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="15"/>
-      <c r="B88" s="11" t="e">
+        <v>2</v>
+      </c>
+      <c r="H87" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="15">
+        <v>45261</v>
+      </c>
+      <c r="B88" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="C88" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D88" s="13">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E88" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F88" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H88" s="16"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="15"/>
-      <c r="B89" s="11" t="e">
+        <v>5.5</v>
+      </c>
+      <c r="H88" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="15">
+        <v>45261</v>
+      </c>
+      <c r="B89" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="C89" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="D89" s="13">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E89" s="30">
+        <v>0</v>
+      </c>
       <c r="F89" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G89" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H89" s="16"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="15"/>
-      <c r="B90" s="11" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="H89" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="15">
+        <v>45263</v>
+      </c>
+      <c r="B90" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C90" s="12"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="C90" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="D90" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="E90" s="30">
+        <v>0</v>
+      </c>
       <c r="F90" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G90" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H90" s="16"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="15"/>
-      <c r="B91" s="11" t="e">
+        <v>3</v>
+      </c>
+      <c r="H90" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="15">
+        <v>45267</v>
+      </c>
+      <c r="B91" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C91" s="12"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="30"/>
+        <v>49</v>
+      </c>
+      <c r="C91" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="D91" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="E91" s="30">
+        <v>0</v>
+      </c>
       <c r="F91" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G91" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H91" s="16"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="H91" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
       <c r="B92" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5016,7 +5077,7 @@
       </c>
       <c r="H92" s="16"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
       <c r="B93" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5035,7 +5096,7 @@
       </c>
       <c r="H93" s="16"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
       <c r="B94" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5054,7 +5115,7 @@
       </c>
       <c r="H94" s="16"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
       <c r="B95" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5073,7 +5134,7 @@
       </c>
       <c r="H95" s="16"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
       <c r="B96" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5092,7 +5153,7 @@
       </c>
       <c r="H96" s="16"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="15"/>
       <c r="B97" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5111,7 +5172,7 @@
       </c>
       <c r="H97" s="16"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
       <c r="B98" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5130,7 +5191,7 @@
       </c>
       <c r="H98" s="16"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
       <c r="B99" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5149,7 +5210,7 @@
       </c>
       <c r="H99" s="16"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="15"/>
       <c r="B100" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5168,7 +5229,7 @@
       </c>
       <c r="H100" s="16"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
       <c r="B101" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5187,7 +5248,7 @@
       </c>
       <c r="H101" s="17"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
       <c r="B102" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5206,7 +5267,7 @@
       </c>
       <c r="H102" s="16"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="15"/>
       <c r="B103" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5225,7 +5286,7 @@
       </c>
       <c r="H103" s="16"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="15"/>
       <c r="B104" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5244,7 +5305,7 @@
       </c>
       <c r="H104" s="16"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="15"/>
       <c r="B105" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5263,7 +5324,7 @@
       </c>
       <c r="H105" s="16"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="15"/>
       <c r="B106" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5282,7 +5343,7 @@
       </c>
       <c r="H106" s="16"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="15"/>
       <c r="B107" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5301,7 +5362,7 @@
       </c>
       <c r="H107" s="16"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="15"/>
       <c r="B108" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5320,7 +5381,7 @@
       </c>
       <c r="H108" s="16"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="15"/>
       <c r="B109" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5339,7 +5400,7 @@
       </c>
       <c r="H109" s="16"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="15"/>
       <c r="B110" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5358,7 +5419,7 @@
       </c>
       <c r="H110" s="16"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="15"/>
       <c r="B111" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5377,7 +5438,7 @@
       </c>
       <c r="H111" s="16"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="15"/>
       <c r="B112" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5396,7 +5457,7 @@
       </c>
       <c r="H112" s="16"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="15"/>
       <c r="B113" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5415,7 +5476,7 @@
       </c>
       <c r="H113" s="16"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="15"/>
       <c r="B114" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5434,7 +5495,7 @@
       </c>
       <c r="H114" s="16"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="15"/>
       <c r="B115" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5453,7 +5514,7 @@
       </c>
       <c r="H115" s="16"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="15"/>
       <c r="B116" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5472,7 +5533,7 @@
       </c>
       <c r="H116" s="16"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="15"/>
       <c r="B117" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5491,7 +5552,7 @@
       </c>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="15"/>
       <c r="B118" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5510,7 +5571,7 @@
       </c>
       <c r="H118" s="16"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="15"/>
       <c r="B119" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5529,7 +5590,7 @@
       </c>
       <c r="H119" s="16"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="15"/>
       <c r="B120" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5548,7 +5609,7 @@
       </c>
       <c r="H120" s="16"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
       <c r="B121" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5567,7 +5628,7 @@
       </c>
       <c r="H121" s="16"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5586,7 +5647,7 @@
       </c>
       <c r="H122" s="16"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5605,7 +5666,7 @@
       </c>
       <c r="H123" s="16"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5624,7 +5685,7 @@
       </c>
       <c r="H124" s="16"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="15"/>
       <c r="B125" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5643,7 +5704,7 @@
       </c>
       <c r="H125" s="16"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
       <c r="B126" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5662,7 +5723,7 @@
       </c>
       <c r="H126" s="16"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="15"/>
       <c r="B127" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5681,7 +5742,7 @@
       </c>
       <c r="H127" s="16"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="15"/>
       <c r="B128" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5700,7 +5761,7 @@
       </c>
       <c r="H128" s="16"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="15"/>
       <c r="B129" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5719,7 +5780,7 @@
       </c>
       <c r="H129" s="16"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="15"/>
       <c r="B130" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5738,7 +5799,7 @@
       </c>
       <c r="H130" s="16"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="15"/>
       <c r="B131" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5757,7 +5818,7 @@
       </c>
       <c r="H131" s="16"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="15"/>
       <c r="B132" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5776,7 +5837,7 @@
       </c>
       <c r="H132" s="16"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="15"/>
       <c r="B133" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5795,7 +5856,7 @@
       </c>
       <c r="H133" s="16"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="15"/>
       <c r="B134" s="11" t="e">
         <f t="shared" ref="B134:B197" si="6">TRUNC((A134-DATE(YEAR(A134+3-MOD(A134-2,7)),1,MOD(A134-2,7)-9))/7)</f>
@@ -5814,7 +5875,7 @@
       </c>
       <c r="H134" s="16"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="15"/>
       <c r="B135" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5833,7 +5894,7 @@
       </c>
       <c r="H135" s="16"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="15"/>
       <c r="B136" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5852,7 +5913,7 @@
       </c>
       <c r="H136" s="16"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="15"/>
       <c r="B137" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5871,7 +5932,7 @@
       </c>
       <c r="H137" s="16"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="15"/>
       <c r="B138" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5890,7 +5951,7 @@
       </c>
       <c r="H138" s="16"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="15"/>
       <c r="B139" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5909,7 +5970,7 @@
       </c>
       <c r="H139" s="16"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="15"/>
       <c r="B140" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5928,7 +5989,7 @@
       </c>
       <c r="H140" s="16"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="15"/>
       <c r="B141" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5947,7 +6008,7 @@
       </c>
       <c r="H141" s="16"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="15"/>
       <c r="B142" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5966,7 +6027,7 @@
       </c>
       <c r="H142" s="16"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="15"/>
       <c r="B143" s="11" t="e">
         <f t="shared" si="6"/>
@@ -5985,7 +6046,7 @@
       </c>
       <c r="H143" s="16"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="15"/>
       <c r="B144" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6004,7 +6065,7 @@
       </c>
       <c r="H144" s="16"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="15"/>
       <c r="B145" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6023,7 +6084,7 @@
       </c>
       <c r="H145" s="16"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="15"/>
       <c r="B146" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6042,7 +6103,7 @@
       </c>
       <c r="H146" s="16"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="15"/>
       <c r="B147" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6061,7 +6122,7 @@
       </c>
       <c r="H147" s="16"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="15"/>
       <c r="B148" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6080,7 +6141,7 @@
       </c>
       <c r="H148" s="16"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="15"/>
       <c r="B149" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6099,7 +6160,7 @@
       </c>
       <c r="H149" s="16"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="15"/>
       <c r="B150" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6118,7 +6179,7 @@
       </c>
       <c r="H150" s="16"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="15"/>
       <c r="B151" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6137,7 +6198,7 @@
       </c>
       <c r="H151" s="16"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="15"/>
       <c r="B152" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6156,7 +6217,7 @@
       </c>
       <c r="H152" s="16"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="15"/>
       <c r="B153" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6175,7 +6236,7 @@
       </c>
       <c r="H153" s="16"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="15"/>
       <c r="B154" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6194,7 +6255,7 @@
       </c>
       <c r="H154" s="16"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="15"/>
       <c r="B155" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6213,7 +6274,7 @@
       </c>
       <c r="H155" s="16"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="15"/>
       <c r="B156" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6232,7 +6293,7 @@
       </c>
       <c r="H156" s="16"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="15"/>
       <c r="B157" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6251,7 +6312,7 @@
       </c>
       <c r="H157" s="16"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="15"/>
       <c r="B158" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6270,7 +6331,7 @@
       </c>
       <c r="H158" s="16"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="15"/>
       <c r="B159" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6289,7 +6350,7 @@
       </c>
       <c r="H159" s="16"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="15"/>
       <c r="B160" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6308,7 +6369,7 @@
       </c>
       <c r="H160" s="16"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="15"/>
       <c r="B161" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6327,7 +6388,7 @@
       </c>
       <c r="H161" s="16"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="15"/>
       <c r="B162" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6346,7 +6407,7 @@
       </c>
       <c r="H162" s="16"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="15"/>
       <c r="B163" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6365,7 +6426,7 @@
       </c>
       <c r="H163" s="16"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="15"/>
       <c r="B164" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6384,7 +6445,7 @@
       </c>
       <c r="H164" s="16"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="15"/>
       <c r="B165" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6403,7 +6464,7 @@
       </c>
       <c r="H165" s="16"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="15"/>
       <c r="B166" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6422,7 +6483,7 @@
       </c>
       <c r="H166" s="16"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="15"/>
       <c r="B167" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6441,7 +6502,7 @@
       </c>
       <c r="H167" s="16"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="15"/>
       <c r="B168" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6460,7 +6521,7 @@
       </c>
       <c r="H168" s="16"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="15"/>
       <c r="B169" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6479,7 +6540,7 @@
       </c>
       <c r="H169" s="16"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="15"/>
       <c r="B170" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6498,7 +6559,7 @@
       </c>
       <c r="H170" s="16"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="15"/>
       <c r="B171" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6517,7 +6578,7 @@
       </c>
       <c r="H171" s="16"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="15"/>
       <c r="B172" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6536,7 +6597,7 @@
       </c>
       <c r="H172" s="16"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="15"/>
       <c r="B173" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6555,7 +6616,7 @@
       </c>
       <c r="H173" s="16"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="15"/>
       <c r="B174" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6574,7 +6635,7 @@
       </c>
       <c r="H174" s="16"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="15"/>
       <c r="B175" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6593,7 +6654,7 @@
       </c>
       <c r="H175" s="16"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="15"/>
       <c r="B176" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6612,7 +6673,7 @@
       </c>
       <c r="H176" s="16"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="15"/>
       <c r="B177" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6631,7 +6692,7 @@
       </c>
       <c r="H177" s="16"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="15"/>
       <c r="B178" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6650,7 +6711,7 @@
       </c>
       <c r="H178" s="16"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="15"/>
       <c r="B179" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6669,7 +6730,7 @@
       </c>
       <c r="H179" s="16"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="15"/>
       <c r="B180" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6688,7 +6749,7 @@
       </c>
       <c r="H180" s="16"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="15"/>
       <c r="B181" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6707,7 +6768,7 @@
       </c>
       <c r="H181" s="16"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="15"/>
       <c r="B182" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6726,7 +6787,7 @@
       </c>
       <c r="H182" s="16"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="15"/>
       <c r="B183" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6745,7 +6806,7 @@
       </c>
       <c r="H183" s="16"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="15"/>
       <c r="B184" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6764,7 +6825,7 @@
       </c>
       <c r="H184" s="16"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="15"/>
       <c r="B185" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6783,7 +6844,7 @@
       </c>
       <c r="H185" s="16"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="15"/>
       <c r="B186" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6802,7 +6863,7 @@
       </c>
       <c r="H186" s="16"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="15"/>
       <c r="B187" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6821,7 +6882,7 @@
       </c>
       <c r="H187" s="16"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="15"/>
       <c r="B188" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6840,7 +6901,7 @@
       </c>
       <c r="H188" s="16"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="15"/>
       <c r="B189" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6859,7 +6920,7 @@
       </c>
       <c r="H189" s="16"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="15"/>
       <c r="B190" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6878,7 +6939,7 @@
       </c>
       <c r="H190" s="16"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="15"/>
       <c r="B191" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6897,7 +6958,7 @@
       </c>
       <c r="H191" s="16"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="15"/>
       <c r="B192" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6916,7 +6977,7 @@
       </c>
       <c r="H192" s="16"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="15"/>
       <c r="B193" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6935,7 +6996,7 @@
       </c>
       <c r="H193" s="16"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="15"/>
       <c r="B194" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6954,7 +7015,7 @@
       </c>
       <c r="H194" s="16"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="15"/>
       <c r="B195" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6973,7 +7034,7 @@
       </c>
       <c r="H195" s="16"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="15"/>
       <c r="B196" s="11" t="e">
         <f t="shared" si="6"/>
@@ -6992,7 +7053,7 @@
       </c>
       <c r="H196" s="16"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="15"/>
       <c r="B197" s="11" t="e">
         <f t="shared" si="6"/>
@@ -7011,7 +7072,7 @@
       </c>
       <c r="H197" s="16"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="15"/>
       <c r="B198" s="11" t="e">
         <f t="shared" ref="B198:B203" si="9">TRUNC((A198-DATE(YEAR(A198+3-MOD(A198-2,7)),1,MOD(A198-2,7)-9))/7)</f>
@@ -7030,7 +7091,7 @@
       </c>
       <c r="H198" s="16"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="15"/>
       <c r="B199" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7049,7 +7110,7 @@
       </c>
       <c r="H199" s="16"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="15"/>
       <c r="B200" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7068,7 +7129,7 @@
       </c>
       <c r="H200" s="16"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="15"/>
       <c r="B201" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7087,7 +7148,7 @@
       </c>
       <c r="H201" s="16"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="15"/>
       <c r="B202" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7106,7 +7167,7 @@
       </c>
       <c r="H202" s="16"/>
     </row>
-    <row r="203" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="18"/>
       <c r="B203" s="11" t="e">
         <f t="shared" si="9"/>
@@ -7158,15 +7219,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.5546875" customWidth="1"/>
-    <col min="3" max="7" width="5.88671875" customWidth="1"/>
-    <col min="8" max="8" width="38.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
+    <col min="3" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
         <v>11</v>
       </c>
@@ -7178,7 +7239,7 @@
       <c r="G1" s="57"/>
       <c r="H1" s="57"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7196,7 +7257,7 @@
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
     </row>
-    <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
@@ -7212,7 +7273,7 @@
       <c r="G3" s="59"/>
       <c r="H3" s="59"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -7220,8 +7281,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>17</v>
       </c>
@@ -7247,7 +7308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <v>42900</v>
       </c>
@@ -7269,7 +7330,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -7279,7 +7340,7 @@
       <c r="G8" s="36"/>
       <c r="H8" s="38"/>
     </row>
-    <row r="9" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="39"/>
       <c r="C9" s="36"/>
@@ -7289,7 +7350,7 @@
       <c r="G9" s="36"/>
       <c r="H9" s="38"/>
     </row>
-    <row r="10" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="35"/>
       <c r="C10" s="36"/>
@@ -7299,7 +7360,7 @@
       <c r="G10" s="36"/>
       <c r="H10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="35"/>
       <c r="C11" s="36"/>
@@ -7309,7 +7370,7 @@
       <c r="G11" s="36"/>
       <c r="H11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="36"/>
@@ -7319,8 +7380,8 @@
       <c r="G12" s="36"/>
       <c r="H12" s="38"/>
     </row>
-    <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
         <v>27</v>
       </c>
@@ -7332,7 +7393,7 @@
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
@@ -7342,7 +7403,7 @@
       <c r="G15" s="52"/>
       <c r="H15" s="53"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -7375,26 +7436,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C8:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="60" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>173.35</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+        <v>189.35</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
@@ -7402,7 +7463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="5">
         <v>16</v>
       </c>
@@ -7411,7 +7472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" s="5">
         <v>17</v>
       </c>
@@ -7420,7 +7481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>18</v>
       </c>
@@ -7429,7 +7490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="5">
         <v>19</v>
       </c>
@@ -7438,7 +7499,7 @@
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="5">
         <v>20</v>
       </c>
@@ -7447,7 +7508,7 @@
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>21</v>
       </c>
@@ -7456,7 +7517,7 @@
         <v>4.583333333333333</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="5">
         <v>22</v>
       </c>
@@ -7465,7 +7526,7 @@
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="5">
         <v>23</v>
       </c>
@@ -7474,7 +7535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="5">
         <v>24</v>
       </c>
@@ -7483,7 +7544,7 @@
         <v>5.6833333333333336</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="5">
         <v>25</v>
       </c>
@@ -7492,7 +7553,7 @@
         <v>1.4833333333333334</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="5">
         <v>26</v>
       </c>
@@ -7501,7 +7562,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="5">
         <v>27</v>
       </c>
@@ -7510,7 +7571,7 @@
         <v>1.9333333333333331</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="5">
         <v>28</v>
       </c>
@@ -7519,7 +7580,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
         <v>29</v>
       </c>
@@ -7528,7 +7589,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="5">
         <v>30</v>
       </c>
@@ -7537,7 +7598,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="5">
         <v>31</v>
       </c>
@@ -7546,7 +7607,7 @@
         <v>1.4333333333333333</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="5">
         <v>32</v>
       </c>
@@ -7555,7 +7616,7 @@
         <v>7.0666666666666673</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="5">
         <v>33</v>
       </c>
@@ -7564,7 +7625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="5">
         <v>34</v>
       </c>
@@ -7573,7 +7634,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
         <v>35</v>
       </c>
@@ -7582,7 +7643,7 @@
         <v>4.2166666666666668</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
         <v>36</v>
       </c>
@@ -7591,7 +7652,7 @@
         <v>11.566666666666666</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
         <v>37</v>
       </c>
@@ -7600,7 +7661,7 @@
         <v>10.216666666666667</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
         <v>38</v>
       </c>
@@ -7609,7 +7670,7 @@
         <v>10.533333333333333</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="5">
         <v>39</v>
       </c>
@@ -7618,7 +7679,7 @@
         <v>7.4166666666666661</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="5">
         <v>40</v>
       </c>
@@ -7627,7 +7688,7 @@
         <v>12.116666666666667</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="5">
         <v>41</v>
       </c>
@@ -7636,7 +7697,7 @@
         <v>10.883333333333333</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="5">
         <v>42</v>
       </c>
@@ -7645,7 +7706,7 @@
         <v>8.8333333333333321</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="5">
         <v>43</v>
       </c>
@@ -7654,7 +7715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" s="5">
         <v>44</v>
       </c>
@@ -7663,7 +7724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="5">
         <v>45</v>
       </c>
@@ -7672,7 +7733,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" s="5">
         <v>46</v>
       </c>
@@ -7681,7 +7742,7 @@
         <v>20.283333333333331</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="5">
         <v>47</v>
       </c>
@@ -7690,25 +7751,25 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="5">
         <v>48</v>
       </c>
       <c r="D43" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C43,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="5">
         <v>49</v>
       </c>
       <c r="D44" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C44,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="5">
         <v>50</v>
       </c>
@@ -7717,7 +7778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="5">
         <v>51</v>
       </c>
@@ -7726,7 +7787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" s="5">
         <v>52</v>
       </c>
@@ -7735,7 +7796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" s="5">
         <v>1</v>
       </c>
@@ -7744,7 +7805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="5">
         <v>2</v>
       </c>
@@ -7754,7 +7815,7 @@
       </c>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="5">
         <v>3</v>
       </c>
@@ -7763,7 +7824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" s="5">
         <v>4</v>
       </c>
@@ -7772,7 +7833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="5">
         <v>5</v>
       </c>
@@ -7781,7 +7842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C53" s="5">
         <v>6</v>
       </c>
@@ -7790,7 +7851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C54" s="5">
         <v>7</v>
       </c>
@@ -7800,7 +7861,7 @@
       </c>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C55" s="5">
         <v>8</v>
       </c>
@@ -7810,7 +7871,7 @@
       </c>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C56" s="5">
         <v>9</v>
       </c>
@@ -7819,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C57" s="5">
         <v>10</v>
       </c>
@@ -7828,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C58" s="5">
         <v>11</v>
       </c>
@@ -7838,7 +7899,7 @@
       </c>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C59" s="5">
         <v>12</v>
       </c>
@@ -7848,7 +7909,7 @@
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C60" s="5">
         <v>13</v>
       </c>
@@ -7857,7 +7918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C61" s="5">
         <v>14</v>
       </c>
@@ -7866,7 +7927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C62" s="5">
         <v>15</v>
       </c>
@@ -7875,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D63" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IMU basic init (from example program for the breakout)
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07D05A9B-8FFA-4979-81B0-D50600C3A690}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62E12D2-1530-4D64-BB71-E8CD4323BD4E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
   <si>
     <t>Name:</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>Dshot600 implementation finished</t>
+  </si>
+  <si>
+    <t>Dshot test in Kombination mit Fernbedienung</t>
+  </si>
+  <si>
+    <t>IMU MPU9250 und BMP280 initialisiert</t>
   </si>
 </sst>
 </file>
@@ -1586,10 +1592,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -2233,8 +2239,8 @@
   <dimension ref="A1:HZ203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H97" sqref="H97"/>
+      <pane ySplit="4" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,11 +2282,11 @@
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>132.4</v>
+        <v>135.9</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>206.35</v>
+        <v>209.85</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -5219,42 +5225,62 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-      <c r="B97" s="11" t="e">
+      <c r="A97" s="15">
+        <v>45295</v>
+      </c>
+      <c r="B97" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C97" s="12"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="C97" s="12">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D97" s="13">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E97" s="30">
+        <v>0</v>
+      </c>
       <c r="F97" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G97" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H97" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="H97" s="16" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-      <c r="B98" s="11" t="e">
+      <c r="A98" s="15">
+        <v>45299</v>
+      </c>
+      <c r="B98" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="30"/>
+        <v>2</v>
+      </c>
+      <c r="C98" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D98" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="E98" s="30">
+        <v>0</v>
+      </c>
       <c r="F98" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G98" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H98" s="16"/>
+        <v>1.5</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
@@ -7517,7 +7543,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>206.35</v>
+        <v>209.85</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -7867,7 +7893,7 @@
       </c>
       <c r="D48" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C48,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -7876,7 +7902,7 @@
       </c>
       <c r="D49" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C49,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G49" s="3"/>
     </row>

</xml_diff>

<commit_message>
added hal include files + PID programmed (not tested)
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="273" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95098EA8-88A8-4ED0-9F98-432906220680}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5CBFA7C-C500-4939-B3B6-90F07360A2CC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="138">
   <si>
     <t>Name:</t>
   </si>
@@ -481,6 +481,18 @@
   </si>
   <si>
     <t>LED Muster erstellen</t>
+  </si>
+  <si>
+    <t>Flight Controller Platine DShot Ausgabe Test</t>
+  </si>
+  <si>
+    <t>PID Einlesen + Flight Controller Platine Test, IMU und Motoren</t>
+  </si>
+  <si>
+    <t>Besprechung Programm flashen + Platinen design</t>
+  </si>
+  <si>
+    <t>PID ausprogrammiert (noch nicht getestet)</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1655,7 @@
                   <c:v>11.166666666666668</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>7.6333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
@@ -2278,8 +2290,8 @@
   <dimension ref="A1:HZ203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
+      <pane ySplit="4" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2317,15 +2329,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>87.45</v>
+        <v>89.95</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>159.98333333333335</v>
+        <v>165.11666666666667</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>247.43333333333334</v>
+        <v>255.06666666666666</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -5728,80 +5740,120 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="15"/>
-      <c r="B113" s="11" t="e">
+      <c r="A113" s="15">
+        <v>45320</v>
+      </c>
+      <c r="B113" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C113" s="12"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="C113" s="12">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D113" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="E113" s="30">
+        <v>0</v>
+      </c>
       <c r="F113" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G113" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H113" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="15"/>
-      <c r="B114" s="11" t="e">
+      <c r="A114" s="15">
+        <v>45321</v>
+      </c>
+      <c r="B114" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C114" s="12"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="C114" s="12">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D114" s="13">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E114" s="30">
+        <v>2.5</v>
+      </c>
       <c r="F114" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.66666666666666652</v>
       </c>
       <c r="G114" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H114" s="16"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="H114" s="16" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="15"/>
-      <c r="B115" s="11" t="e">
+      <c r="A115" s="15">
+        <v>45322</v>
+      </c>
+      <c r="B115" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C115" s="12"/>
-      <c r="D115" s="13"/>
-      <c r="E115" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="C115" s="12">
+        <v>0.77222222222222225</v>
+      </c>
+      <c r="D115" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="E115" s="30">
+        <v>0</v>
+      </c>
       <c r="F115" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.4666666666666668</v>
       </c>
       <c r="G115" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H115" s="16"/>
+        <v>2.4666666666666668</v>
+      </c>
+      <c r="H115" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
-      <c r="B116" s="11" t="e">
+      <c r="A116" s="15">
+        <v>45323</v>
+      </c>
+      <c r="B116" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="C116" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D116" s="13">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E116" s="30">
+        <v>0</v>
+      </c>
       <c r="F116" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G116" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H116" s="16"/>
+        <v>1.5</v>
+      </c>
+      <c r="H116" s="16" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="15"/>
@@ -7722,7 +7774,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>247.43333333333331</v>
+        <v>255.06666666666663</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -8109,7 +8161,7 @@
       </c>
       <c r="D52" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C52,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>0</v>
+        <v>7.6333333333333329</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -8222,6 +8274,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -8353,12 +8411,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8369,6 +8421,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8386,15 +8447,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
better comments + improvments
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5CBFA7C-C500-4939-B3B6-90F07360A2CC}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ABADDF4-ECA5-42B5-9B39-4DD37174A995}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="140">
   <si>
     <t>Name:</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>PID ausprogrammiert (noch nicht getestet)</t>
+  </si>
+  <si>
+    <t>Flight Controller Platine IMU-, DS2438-, Motortest</t>
+  </si>
+  <si>
+    <t>IMU + Data transmission tests</t>
   </si>
 </sst>
 </file>
@@ -1655,10 +1661,10 @@
                   <c:v>11.166666666666668</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.6333333333333329</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0</c:v>
@@ -2291,7 +2297,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
+      <selection pane="bottomLeft" activeCell="H119" sqref="H119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,15 +2335,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>89.95</v>
+        <v>94.45</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>165.11666666666667</v>
+        <v>168.53333333333333</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>255.06666666666666</v>
+        <v>262.98333333333335</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -5856,42 +5862,62 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="15"/>
-      <c r="B117" s="11" t="e">
+      <c r="A117" s="15">
+        <v>45324</v>
+      </c>
+      <c r="B117" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C117" s="12"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="C117" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D117" s="13">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E117" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F117" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="G117" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H117" s="16"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H117" s="16" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="15"/>
-      <c r="B118" s="11" t="e">
+      <c r="A118" s="15">
+        <v>45327</v>
+      </c>
+      <c r="B118" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C118" s="12"/>
-      <c r="D118" s="13"/>
-      <c r="E118" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="C118" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D118" s="13">
+        <v>0.46875</v>
+      </c>
+      <c r="E118" s="30">
+        <v>0</v>
+      </c>
       <c r="F118" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G118" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H118" s="16"/>
+        <v>1.25</v>
+      </c>
+      <c r="H118" s="16" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="15"/>
@@ -7774,7 +7800,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>255.06666666666663</v>
+        <v>262.98333333333329</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -8161,7 +8187,7 @@
       </c>
       <c r="D52" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C52,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>7.6333333333333329</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -8170,7 +8196,7 @@
       </c>
       <c r="D53" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C53,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Doku DS2438 fast fertig + IMU angefangen
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BCA549C-131A-46E8-ABF6-D5AF355AECF1}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1E5F3EE-B957-4AD3-85A1-3F7F9FFD4DD4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
   <si>
     <t>Name:</t>
   </si>
@@ -511,6 +511,24 @@
   </si>
   <si>
     <t>Dokumentation PID, Lagewinkel, IMU weiterschreiben</t>
+  </si>
+  <si>
+    <t>Dokumentation DS2438 anfangen</t>
+  </si>
+  <si>
+    <t>Drohnen SW- / HW- / Flugtests</t>
+  </si>
+  <si>
+    <t>Datenübertragung + PID-Tests</t>
+  </si>
+  <si>
+    <t>Doku DS2438</t>
+  </si>
+  <si>
+    <t>Doku DS2438, IMU, Fernsteuerung</t>
+  </si>
+  <si>
+    <t>Doku IMU, MPU9250 + BMP280</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1694,10 @@
                   <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.5666666666666664</c:v>
+                  <c:v>18.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>14.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -2308,8 +2326,8 @@
   <dimension ref="A1:HZ203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
+      <pane ySplit="4" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,15 +2365,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>94.45</v>
+        <v>98.95</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>175.85</v>
+        <v>196.43333333333331</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>270.3</v>
+        <v>295.38333333333338</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -6048,118 +6066,178 @@
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="15"/>
-      <c r="B123" s="11" t="e">
+      <c r="A123" s="15">
+        <v>45329</v>
+      </c>
+      <c r="B123" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C123" s="12"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="C123" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D123" s="13">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E123" s="30">
+        <v>0</v>
+      </c>
       <c r="F123" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G123" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H123" s="16"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="H123" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="15"/>
-      <c r="B124" s="11" t="e">
+      <c r="A124" s="15">
+        <v>45331</v>
+      </c>
+      <c r="B124" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C124" s="12"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="C124" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D124" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E124" s="30">
+        <v>0</v>
+      </c>
       <c r="F124" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G124" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H124" s="16"/>
+        <v>9</v>
+      </c>
+      <c r="H124" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="15"/>
-      <c r="B125" s="11" t="e">
+      <c r="A125" s="15">
+        <v>45338</v>
+      </c>
+      <c r="B125" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C125" s="12"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="C125" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D125" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E125" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F125" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.6666666666666661</v>
       </c>
       <c r="G125" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H125" s="16"/>
+        <v>8.1666666666666661</v>
+      </c>
+      <c r="H125" s="16" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="15"/>
-      <c r="B126" s="11" t="e">
+      <c r="A126" s="15">
+        <v>45339</v>
+      </c>
+      <c r="B126" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C126" s="12"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="C126" s="12">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D126" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E126" s="30">
+        <v>0</v>
+      </c>
       <c r="F126" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G126" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H126" s="16"/>
+        <v>1.5</v>
+      </c>
+      <c r="H126" s="16" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="15"/>
-      <c r="B127" s="11" t="e">
+      <c r="A127" s="15">
+        <v>45339</v>
+      </c>
+      <c r="B127" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C127" s="12"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="C127" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D127" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E127" s="30">
+        <v>0</v>
+      </c>
       <c r="F127" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="G127" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H127" s="16"/>
+        <v>3.5</v>
+      </c>
+      <c r="H127" s="16" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="15"/>
-      <c r="B128" s="11" t="e">
+      <c r="A128" s="15">
+        <v>45340</v>
+      </c>
+      <c r="B128" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C128" s="12"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="C128" s="12">
+        <v>0.59375</v>
+      </c>
+      <c r="D128" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E128" s="30">
+        <v>0</v>
+      </c>
       <c r="F128" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="G128" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H128" s="16"/>
+        <v>1.75</v>
+      </c>
+      <c r="H128" s="16" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="15"/>
@@ -7836,7 +7914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C8:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
@@ -7852,7 +7930,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>270.29999999999995</v>
+        <v>295.38333333333333</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -8248,7 +8326,7 @@
       </c>
       <c r="D53" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C53,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>8.5666666666666664</v>
+        <v>18.733333333333334</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
@@ -8257,7 +8335,7 @@
       </c>
       <c r="D54" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C54,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>0</v>
+        <v>14.916666666666666</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -8352,6 +8430,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -8483,12 +8567,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8499,6 +8577,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8516,15 +8603,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Doku stand 24.02. + changeKs Programm
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C357E9C-D43B-46CD-B679-C3BD17743ECF}"/>
+  <xr:revisionPtr revIDLastSave="407" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D30418-AC5E-42BC-BA7B-DE644287C0DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="155">
   <si>
     <t>Name:</t>
   </si>
@@ -532,6 +532,18 @@
   </si>
   <si>
     <t>Doku IMU + Software Blockschaltbild</t>
+  </si>
+  <si>
+    <t>Testen Datenübertragung + neuen PID-Regler</t>
+  </si>
+  <si>
+    <t>Doku PID-Regler</t>
+  </si>
+  <si>
+    <t>Doku schreiben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doku schreiben </t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1715,7 @@
                   <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>0</c:v>
@@ -2329,8 +2341,8 @@
   <dimension ref="A1:HZ203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
+      <pane ySplit="4" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H134" sqref="H134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,15 +2380,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>97.95</v>
+        <v>102.45</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>198.26666666666665</v>
+        <v>208.26666666666665</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>296.2166666666667</v>
+        <v>310.7166666666667</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -6272,82 +6284,120 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="15"/>
-      <c r="B130" s="11" t="e">
+      <c r="A130" s="15">
+        <v>45345</v>
+      </c>
+      <c r="B130" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C130" s="12"/>
-      <c r="D130" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="C130" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D130" s="13">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E130" s="30">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F130" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.6666666666666661</v>
       </c>
       <c r="G130" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H130" s="16"/>
+        <v>8.1666666666666661</v>
+      </c>
+      <c r="H130" s="16" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="15"/>
-      <c r="B131" s="11" t="e">
+      <c r="A131" s="15">
+        <v>45345</v>
+      </c>
+      <c r="B131" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C131" s="12"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="30"/>
+        <v>8</v>
+      </c>
+      <c r="C131" s="12">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D131" s="13">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E131" s="30">
+        <v>0</v>
+      </c>
       <c r="F131" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="G131" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H131" s="16"/>
+        <v>2.25</v>
+      </c>
+      <c r="H131" s="16" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="15"/>
-      <c r="B132" s="11" t="e">
+      <c r="A132" s="15">
+        <v>45346</v>
+      </c>
+      <c r="B132" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C132" s="12"/>
-      <c r="D132" s="13"/>
-      <c r="E132" s="30"/>
+        <v>8</v>
+      </c>
+      <c r="C132" s="12">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D132" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E132" s="30">
+        <v>0</v>
+      </c>
       <c r="F132" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="G132" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H132" s="16"/>
+        <v>2.25</v>
+      </c>
+      <c r="H132" s="16" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="15"/>
-      <c r="B133" s="11" t="e">
+      <c r="A133" s="15">
+        <v>45346</v>
+      </c>
+      <c r="B133" s="11">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C133" s="12"/>
-      <c r="D133" s="13"/>
-      <c r="E133" s="30"/>
+        <v>8</v>
+      </c>
+      <c r="C133" s="12">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D133" s="13">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E133" s="30">
+        <v>0</v>
+      </c>
       <c r="F133" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.8333333333333335</v>
       </c>
       <c r="G133" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H133" s="16"/>
+        <v>1.8333333333333335</v>
+      </c>
+      <c r="H133" s="16" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="15"/>
@@ -7945,7 +7995,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>296.21666666666664</v>
+        <v>310.71666666666664</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -8360,7 +8410,7 @@
       </c>
       <c r="D55" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C55,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="G55" s="3"/>
     </row>

</xml_diff>

<commit_message>
new program structure V1 + Doku Stand 26.02.
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="407" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D30418-AC5E-42BC-BA7B-DE644287C0DB}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA148FAD-B8F8-4C3C-A795-181E89F78F60}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
   <si>
     <t>Name:</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t xml:space="preserve">Doku schreiben </t>
+  </si>
+  <si>
+    <t>Programm: Regler Koeffizienten über UART ändern + Doku</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1721,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0</c:v>
@@ -2342,7 +2345,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H134" sqref="H134"/>
+      <selection pane="bottomLeft" activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,11 +2387,11 @@
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>208.26666666666665</v>
+        <v>212.26666666666665</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>310.7166666666667</v>
+        <v>314.7166666666667</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -6400,23 +6403,33 @@
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="15"/>
-      <c r="B134" s="11" t="e">
+      <c r="A134" s="15">
+        <v>45348</v>
+      </c>
+      <c r="B134" s="11">
         <f t="shared" ref="B134:B197" si="6">TRUNC((A134-DATE(YEAR(A134+3-MOD(A134-2,7)),1,MOD(A134-2,7)-9))/7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C134" s="12"/>
-      <c r="D134" s="13"/>
-      <c r="E134" s="30"/>
+        <v>9</v>
+      </c>
+      <c r="C134" s="12">
+        <v>0.78125</v>
+      </c>
+      <c r="D134" s="13">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E134" s="30">
+        <v>0</v>
+      </c>
       <c r="F134" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G134" s="29">
         <f t="shared" ref="G134:G197" si="7">HOUR($D134-$C134)+MINUTE($D134-$C134)/60</f>
-        <v>0</v>
-      </c>
-      <c r="H134" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="H134" s="16" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="15"/>
@@ -7995,7 +8008,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>310.71666666666664</v>
+        <v>314.71666666666664</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -8420,7 +8433,7 @@
       </c>
       <c r="D56" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C56,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
@@ -8495,6 +8508,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -8626,12 +8645,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8642,6 +8655,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8659,15 +8681,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update excel stand 16.03.
</commit_message>
<xml_diff>
--- a/DA_Protokoll_Lendl.xlsx
+++ b/DA_Protokoll_Lendl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c488799b3f1ed5d8/Schule/DA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="497" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95588402-9D8C-4944-89A5-ADB89D280CB0}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="13_ncr:1_{A8ECC070-3A7C-47D9-8D1C-0C4631834678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E41C1D3-8598-465D-A55C-BE1DEB45F566}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="161">
   <si>
     <t>Name:</t>
   </si>
@@ -1745,7 +1745,7 @@
                   <c:v>11.583333333333332</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>0</c:v>
@@ -2370,7 +2370,7 @@
                   <c:v>11.583333333333332</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0</c:v>
@@ -3636,7 +3636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H142" sqref="H142"/>
+      <selection pane="bottomLeft" activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3674,15 +3674,15 @@
       <c r="D2" s="43"/>
       <c r="E2" s="25">
         <f>SUM(E5:E203)</f>
-        <v>115.7</v>
+        <v>120.2</v>
       </c>
       <c r="F2" s="25">
         <f>SUM(F5:F203)</f>
-        <v>233.26666666666665</v>
+        <v>235.43333333333331</v>
       </c>
       <c r="G2" s="26">
         <f>SUM(G5:G203)</f>
-        <v>348.9666666666667</v>
+        <v>355.63333333333338</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -7926,23 +7926,33 @@
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="15"/>
-      <c r="B142" s="11" t="e">
+      <c r="A142" s="15">
+        <v>45367</v>
+      </c>
+      <c r="B142" s="11">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C142" s="12"/>
-      <c r="D142" s="13"/>
-      <c r="E142" s="30"/>
+        <v>11</v>
+      </c>
+      <c r="C142" s="12">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="D142" s="13">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E142" s="30">
+        <v>4.5</v>
+      </c>
       <c r="F142" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="G142" s="29">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H142" s="16"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H142" s="16" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="15"/>
@@ -9369,7 +9379,7 @@
       <c r="D8" s="60"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>348.96666666666664</v>
+        <v>355.63333333333333</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -9812,7 +9822,7 @@
       </c>
       <c r="D58" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C58,Begleitprotokoll!$G$5:$G$200)</f>
-        <v>0</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="H58" s="3"/>
     </row>
@@ -9869,6 +9879,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AD3FA76C40FF345BCA2C97F0BEA1033" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6e2041eff58548933a715487819fb45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c4e4a9d82cce5acc818b14ed3d250e3" ns2:_="">
     <xsd:import namespace="7adf83ab-5e43-45ba-a22e-7b0fb05f9f24"/>
@@ -10000,22 +10025,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F572FB-58D1-445D-A923-50F6D2D61375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10031,21 +10058,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4D141D-07A0-4E53-A884-D40FAAA8E67D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E0995F-5523-464E-96ED-BF1A4901DFD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>